<commit_message>
Add social_security_data SAS file and load into SAS EGP project.
</commit_message>
<xml_diff>
--- a/AgeGroups.xlsx
+++ b/AgeGroups.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Field Breakdown" sheetId="1" r:id="rId1"/>
+    <sheet name="ID Lookup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
   <si>
     <t>Disease_Cases</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>15 to 44 years</t>
+  </si>
+  <si>
+    <t>both sexes</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
   <si>
     <t>AgeGroup</t>
@@ -596,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,9 +617,12 @@
     <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,8 +635,17 @@
       <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -637,8 +658,17 @@
       <c r="D2" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -651,8 +681,17 @@
       <c r="D3" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -665,8 +704,17 @@
       <c r="D4" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -680,7 +728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -694,7 +742,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -708,7 +756,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -722,7 +770,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -733,7 +781,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
@@ -741,7 +789,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
@@ -749,7 +797,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -757,7 +805,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -765,15 +813,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -781,7 +832,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -874,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,13 +938,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -915,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -926,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -937,7 +988,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -948,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -959,7 +1010,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -970,7 +1021,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -981,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -992,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1003,7 +1054,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1014,7 +1065,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1025,7 +1076,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1036,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1047,7 +1098,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1058,7 +1109,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1069,7 +1120,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1080,7 +1131,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1091,7 +1142,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1102,7 +1153,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1113,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1124,7 +1175,7 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1135,7 +1186,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1146,7 +1197,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1157,7 +1208,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>